<commit_message>
se avanzo un poco en el marco teorico del documento
</commit_message>
<xml_diff>
--- a/img/Libro1.xlsx
+++ b/img/Libro1.xlsx
@@ -3,10 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="graficas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="graficas +" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
   <extLst>
@@ -16,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">solcuion para assigments (X)</t>
   </si>
@@ -76,6 +78,45 @@
   </si>
   <si>
     <t>x_p2</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>Trechos</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>1-3</t>
+  </si>
+  <si>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>1-5</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>2-4</t>
+  </si>
+  <si>
+    <t>2-5</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>3-5</t>
+  </si>
+  <si>
+    <t>4-5</t>
   </si>
 </sst>
 </file>
@@ -85,15 +126,27 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16.000000"/>
+      <color theme="0" tint="0"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -109,8 +162,26 @@
         <bgColor theme="9" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="0"/>
+        <bgColor theme="0" tint="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.499984740745262"/>
+        <bgColor theme="8" tint="-0.499984740745262"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor theme="8" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="8">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -142,12 +213,69 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="0" applyFill="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="31">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -172,6 +300,48 @@
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf fontId="0" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="4" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="5" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="3" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="5" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="5" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="2" fillId="5" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="7" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="2" fillId="5" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="6" borderId="1" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="4" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,6 +358,110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>145647</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457718</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>56165</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2661924" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1974447" y="904875"/>
+          <a:ext cx="312069" cy="237140"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="t" anchorCtr="0" forceAA="0" upright="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape"/>
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:p>
+          <a:pPr algn="ctr">
+            <a:defRPr/>
+          </a:pPr>
+          <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+            <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+              <a14:m>
+                <m:oMathPara>
+                  <m:oMathParaPr/>
+                  <m:oMath>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr i="1">
+                            <a:latin typeface="Cambria Math"/>
+                            <a:ea typeface="Cambria Math"/>
+                            <a:cs typeface="Cambria Math"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="i"/>
+                          </m:rPr>
+                          <a:rPr>
+                            <a:latin typeface="Cambria Math"/>
+                            <a:ea typeface="Cambria Math"/>
+                            <a:cs typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>E</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="i"/>
+                          </m:rPr>
+                          <a:rPr>
+                            <a:latin typeface="Cambria Math"/>
+                            <a:ea typeface="Cambria Math"/>
+                            <a:cs typeface="Cambria Math"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+            </mc:Choice>
+            <mc:Fallback/>
+          </mc:AlternateContent>
+          <a:endParaRPr>
+            <a:latin typeface="Cambria Math"/>
+            <a:ea typeface="Cambria Math"/>
+            <a:cs typeface="Cambria Math"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1277,4 +1551,831 @@
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="1" topLeftCell="D1" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="1.8515625"/>
+    <col bestFit="1" min="3" max="3" style="13" width="10.32421875"/>
+    <col customWidth="1" min="4" max="4" style="13" width="1.1328125"/>
+    <col customWidth="1" min="5" max="5" width="5.8515625"/>
+    <col customWidth="1" min="6" max="7" width="5.7109375"/>
+    <col customWidth="1" min="8" max="8" width="1.1328125"/>
+    <col customWidth="1" min="9" max="11" width="5.7109375"/>
+    <col customWidth="1" min="12" max="12" width="1.7109375"/>
+    <col customWidth="1" min="14" max="14" width="1.54296875"/>
+    <col bestFit="1" min="15" max="15" width="10.32421875"/>
+    <col customWidth="1" min="16" max="16" width="1.1328125"/>
+    <col customWidth="1" min="17" max="19" width="5.7109375"/>
+    <col customWidth="1" min="20" max="20" width="1.2109375"/>
+    <col customWidth="1" min="21" max="23" width="5.7109375"/>
+    <col customWidth="1" min="24" max="24" width="1.3828125"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="8.25" customHeight="1">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="14"/>
+    </row>
+    <row r="3" ht="21">
+      <c r="B3" s="14"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="R3" s="22"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="V3" s="22"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="14"/>
+    </row>
+    <row r="4" ht="21">
+      <c r="B4" s="14"/>
+      <c r="C4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="14"/>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18">
+        <v>2</v>
+      </c>
+      <c r="G4" s="18">
+        <v>3</v>
+      </c>
+      <c r="H4" s="14"/>
+      <c r="I4" s="18">
+        <v>1</v>
+      </c>
+      <c r="J4" s="18">
+        <v>2</v>
+      </c>
+      <c r="K4" s="18">
+        <v>3</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="18">
+        <v>1</v>
+      </c>
+      <c r="R4" s="18">
+        <v>2</v>
+      </c>
+      <c r="S4" s="18">
+        <v>3</v>
+      </c>
+      <c r="T4" s="24"/>
+      <c r="U4" s="18">
+        <v>1</v>
+      </c>
+      <c r="V4" s="18">
+        <v>2</v>
+      </c>
+      <c r="W4" s="18">
+        <v>3</v>
+      </c>
+      <c r="X4" s="14"/>
+    </row>
+    <row r="5" ht="21">
+      <c r="B5" s="14"/>
+      <c r="C5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="14"/>
+      <c r="E5" s="27">
+        <v>145</v>
+      </c>
+      <c r="F5" s="27">
+        <v>116</v>
+      </c>
+      <c r="G5" s="27">
+        <v>55</v>
+      </c>
+      <c r="H5" s="14"/>
+      <c r="I5" s="27">
+        <v>127</v>
+      </c>
+      <c r="J5" s="27">
+        <v>52</v>
+      </c>
+      <c r="K5" s="27">
+        <v>0</v>
+      </c>
+      <c r="L5" s="14"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="27">
+        <v>29</v>
+      </c>
+      <c r="R5" s="27">
+        <v>61</v>
+      </c>
+      <c r="S5" s="27">
+        <v>55</v>
+      </c>
+      <c r="T5" s="24"/>
+      <c r="U5" s="27">
+        <v>75</v>
+      </c>
+      <c r="V5" s="27">
+        <v>52</v>
+      </c>
+      <c r="W5" s="27">
+        <v>0</v>
+      </c>
+      <c r="X5" s="14"/>
+    </row>
+    <row r="6" ht="21">
+      <c r="B6" s="14"/>
+      <c r="C6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="14"/>
+      <c r="E6" s="27">
+        <v>52</v>
+      </c>
+      <c r="F6" s="27">
+        <v>40</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14"/>
+      <c r="I6" s="27">
+        <v>0</v>
+      </c>
+      <c r="J6" s="27">
+        <v>0</v>
+      </c>
+      <c r="K6" s="27">
+        <v>0</v>
+      </c>
+      <c r="L6" s="14"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="27">
+        <v>12</v>
+      </c>
+      <c r="R6" s="27">
+        <v>40</v>
+      </c>
+      <c r="S6" s="27">
+        <v>0</v>
+      </c>
+      <c r="T6" s="24"/>
+      <c r="U6" s="27">
+        <v>0</v>
+      </c>
+      <c r="V6" s="27">
+        <v>0</v>
+      </c>
+      <c r="W6" s="27">
+        <v>0</v>
+      </c>
+      <c r="X6" s="14"/>
+    </row>
+    <row r="7" ht="21">
+      <c r="B7" s="14"/>
+      <c r="C7" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="27">
+        <v>0</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14"/>
+      <c r="I7" s="27">
+        <v>0</v>
+      </c>
+      <c r="J7" s="27">
+        <v>0</v>
+      </c>
+      <c r="K7" s="27">
+        <v>0</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="27">
+        <v>0</v>
+      </c>
+      <c r="R7" s="27">
+        <v>0</v>
+      </c>
+      <c r="S7" s="27">
+        <v>0</v>
+      </c>
+      <c r="T7" s="24"/>
+      <c r="U7" s="27">
+        <v>0</v>
+      </c>
+      <c r="V7" s="27">
+        <v>0</v>
+      </c>
+      <c r="W7" s="27">
+        <v>0</v>
+      </c>
+      <c r="X7" s="14"/>
+    </row>
+    <row r="8" ht="21">
+      <c r="B8" s="14"/>
+      <c r="C8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="14"/>
+      <c r="E8" s="27">
+        <v>0</v>
+      </c>
+      <c r="F8" s="27">
+        <v>0</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14"/>
+      <c r="I8" s="27">
+        <v>0</v>
+      </c>
+      <c r="J8" s="27">
+        <v>0</v>
+      </c>
+      <c r="K8" s="27">
+        <v>0</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="24"/>
+      <c r="Q8" s="27">
+        <v>0</v>
+      </c>
+      <c r="R8" s="27">
+        <v>0</v>
+      </c>
+      <c r="S8" s="27">
+        <v>0</v>
+      </c>
+      <c r="T8" s="24"/>
+      <c r="U8" s="27">
+        <v>0</v>
+      </c>
+      <c r="V8" s="27">
+        <v>0</v>
+      </c>
+      <c r="W8" s="27">
+        <v>0</v>
+      </c>
+      <c r="X8" s="14"/>
+    </row>
+    <row r="9" ht="6" customHeight="1">
+      <c r="B9" s="14"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="29"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="14"/>
+    </row>
+    <row r="10" ht="21">
+      <c r="B10" s="14"/>
+      <c r="C10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="27">
+        <v>128</v>
+      </c>
+      <c r="F10" s="27">
+        <v>104</v>
+      </c>
+      <c r="G10" s="27">
+        <v>63</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="27">
+        <v>80</v>
+      </c>
+      <c r="J10" s="27">
+        <v>51</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="27">
+        <v>24</v>
+      </c>
+      <c r="R10" s="27">
+        <v>41</v>
+      </c>
+      <c r="S10" s="27">
+        <v>63</v>
+      </c>
+      <c r="T10" s="24"/>
+      <c r="U10" s="27">
+        <v>29</v>
+      </c>
+      <c r="V10" s="27">
+        <v>51</v>
+      </c>
+      <c r="W10" s="27">
+        <v>0</v>
+      </c>
+      <c r="X10" s="14"/>
+    </row>
+    <row r="11" ht="21">
+      <c r="B11" s="14"/>
+      <c r="C11" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="27">
+        <v>16</v>
+      </c>
+      <c r="F11" s="27">
+        <v>0</v>
+      </c>
+      <c r="G11" s="27">
+        <v>0</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="27">
+        <v>35</v>
+      </c>
+      <c r="J11" s="27">
+        <v>0</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="27">
+        <v>16</v>
+      </c>
+      <c r="R11" s="27">
+        <v>0</v>
+      </c>
+      <c r="S11" s="27">
+        <v>0</v>
+      </c>
+      <c r="T11" s="24"/>
+      <c r="U11" s="27">
+        <v>35</v>
+      </c>
+      <c r="V11" s="27">
+        <v>0</v>
+      </c>
+      <c r="W11" s="27">
+        <v>0</v>
+      </c>
+      <c r="X11" s="14"/>
+    </row>
+    <row r="12" ht="21">
+      <c r="B12" s="14"/>
+      <c r="C12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="14"/>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>0</v>
+      </c>
+      <c r="G12" s="27">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14"/>
+      <c r="I12" s="27">
+        <v>0</v>
+      </c>
+      <c r="J12" s="27">
+        <v>0</v>
+      </c>
+      <c r="K12" s="27">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="27">
+        <v>0</v>
+      </c>
+      <c r="R12" s="27">
+        <v>0</v>
+      </c>
+      <c r="S12" s="27">
+        <v>0</v>
+      </c>
+      <c r="T12" s="24"/>
+      <c r="U12" s="27">
+        <v>0</v>
+      </c>
+      <c r="V12" s="27">
+        <v>0</v>
+      </c>
+      <c r="W12" s="27">
+        <v>0</v>
+      </c>
+      <c r="X12" s="14"/>
+    </row>
+    <row r="13" ht="5.25" customHeight="1">
+      <c r="B13" s="14"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="30"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="30"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="30"/>
+      <c r="V13" s="30"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="14"/>
+    </row>
+    <row r="14" ht="21">
+      <c r="B14" s="14"/>
+      <c r="C14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="14"/>
+      <c r="E14" s="27">
+        <v>43</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0</v>
+      </c>
+      <c r="H14" s="14"/>
+      <c r="I14" s="27">
+        <v>105</v>
+      </c>
+      <c r="J14" s="27">
+        <v>46</v>
+      </c>
+      <c r="K14" s="27">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14"/>
+      <c r="N14" s="20"/>
+      <c r="O14" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="24"/>
+      <c r="Q14" s="27">
+        <v>43</v>
+      </c>
+      <c r="R14" s="27">
+        <v>0</v>
+      </c>
+      <c r="S14" s="27">
+        <v>0</v>
+      </c>
+      <c r="T14" s="24"/>
+      <c r="U14" s="27">
+        <v>59</v>
+      </c>
+      <c r="V14" s="27">
+        <v>46</v>
+      </c>
+      <c r="W14" s="27">
+        <v>0</v>
+      </c>
+      <c r="X14" s="14"/>
+    </row>
+    <row r="15" ht="21">
+      <c r="B15" s="14"/>
+      <c r="C15" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="14"/>
+      <c r="E15" s="27">
+        <v>85</v>
+      </c>
+      <c r="F15" s="27">
+        <v>59</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="27">
+        <v>88</v>
+      </c>
+      <c r="J15" s="27">
+        <v>4</v>
+      </c>
+      <c r="K15" s="27">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="27">
+        <v>26</v>
+      </c>
+      <c r="R15" s="27">
+        <v>59</v>
+      </c>
+      <c r="S15" s="27">
+        <v>0</v>
+      </c>
+      <c r="T15" s="24"/>
+      <c r="U15" s="27">
+        <v>84</v>
+      </c>
+      <c r="V15" s="27">
+        <v>4</v>
+      </c>
+      <c r="W15" s="27">
+        <v>0</v>
+      </c>
+      <c r="X15" s="14"/>
+    </row>
+    <row r="16" ht="6" customHeight="1">
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="14"/>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
+    </row>
+    <row r="17" ht="21">
+      <c r="B17" s="14"/>
+      <c r="C17" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="27">
+        <v>150</v>
+      </c>
+      <c r="F17" s="27">
+        <v>62</v>
+      </c>
+      <c r="G17" s="27">
+        <v>0</v>
+      </c>
+      <c r="H17" s="14"/>
+      <c r="I17" s="27">
+        <v>143</v>
+      </c>
+      <c r="J17" s="27">
+        <v>58</v>
+      </c>
+      <c r="K17" s="27">
+        <v>0</v>
+      </c>
+      <c r="L17" s="14"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="27">
+        <v>88</v>
+      </c>
+      <c r="R17" s="27">
+        <v>36</v>
+      </c>
+      <c r="S17" s="27">
+        <v>0</v>
+      </c>
+      <c r="T17" s="24"/>
+      <c r="U17" s="27">
+        <v>85</v>
+      </c>
+      <c r="V17" s="27">
+        <v>0</v>
+      </c>
+      <c r="W17" s="27">
+        <v>0</v>
+      </c>
+      <c r="X17" s="14"/>
+    </row>
+    <row r="18" ht="6.75" customHeight="1">
+      <c r="B18" s="14"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
+    </row>
+    <row r="19" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="U3:W3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="E5:G8 I5:K8 E10:G12 I10:K12 E14:G15 E17:G17 I14:K15 I17:K17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q5:S8 U5:W8 Q10:S12 U10:W12 Q14:S15 Q17:S17 U14:W15 U17:W17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4"/>
+    <row r="8">
+      <c r="G8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="G9">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="G10">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="G11">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>